<commit_message>
corrigido bug no AL que não incrementava ponteiro ao analisar os operadores de atribuição e corrigido a gramatica para o print que aceita Expr_star
</commit_message>
<xml_diff>
--- a/src/testes/TabelaSLR_Debug.xlsx
+++ b/src/testes/TabelaSLR_Debug.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2430" windowWidth="14340" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="3645" windowWidth="14340" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="244">
   <si>
     <t>S19</t>
   </si>
@@ -759,9 +759,6 @@
   </si>
   <si>
     <t>ebin</t>
-  </si>
-  <si>
-    <t>R58 corrigido</t>
   </si>
 </sst>
 </file>
@@ -816,12 +813,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1144,10 +1138,10 @@
   <dimension ref="A1:CG172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AX3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BF4" sqref="BF4:BF176"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,431 +1150,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AS1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AV1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AW1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AX1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AY1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BA1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BB1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BC1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BD1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BE1" s="2" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>5</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>6</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>7</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>8</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>9</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>11</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>12</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>13</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>14</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>15</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>16</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>17</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="2">
         <v>18</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="2">
         <v>19</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="2">
         <v>20</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="2">
         <v>21</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="2">
         <v>22</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="2">
         <v>23</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="2">
         <v>24</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AA2" s="2">
         <v>25</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="2">
         <v>26</v>
       </c>
-      <c r="AC2" s="3">
+      <c r="AC2" s="2">
         <v>27</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AD2" s="2">
         <v>28</v>
       </c>
-      <c r="AE2" s="3">
+      <c r="AE2" s="2">
         <v>29</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AF2" s="2">
         <v>30</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AG2" s="2">
         <v>31</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AH2" s="2">
         <v>32</v>
       </c>
-      <c r="AI2" s="3">
+      <c r="AI2" s="2">
         <v>33</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AJ2" s="2">
         <v>34</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AK2" s="2">
         <v>35</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AL2" s="2">
         <v>36</v>
       </c>
-      <c r="AM2" s="3">
+      <c r="AM2" s="2">
         <v>37</v>
       </c>
-      <c r="AN2" s="3">
+      <c r="AN2" s="2">
         <v>38</v>
       </c>
-      <c r="AO2" s="3">
+      <c r="AO2" s="2">
         <v>39</v>
       </c>
-      <c r="AP2" s="3">
+      <c r="AP2" s="2">
         <v>40</v>
       </c>
-      <c r="AQ2" s="3">
+      <c r="AQ2" s="2">
         <v>41</v>
       </c>
-      <c r="AR2" s="3">
+      <c r="AR2" s="2">
         <v>42</v>
       </c>
-      <c r="AS2" s="3">
+      <c r="AS2" s="2">
         <v>43</v>
       </c>
-      <c r="AT2" s="3">
+      <c r="AT2" s="2">
         <v>44</v>
       </c>
-      <c r="AU2" s="3">
+      <c r="AU2" s="2">
         <v>45</v>
       </c>
-      <c r="AV2" s="3">
+      <c r="AV2" s="2">
         <v>46</v>
       </c>
-      <c r="AW2" s="3">
+      <c r="AW2" s="2">
         <v>47</v>
       </c>
-      <c r="AX2" s="3">
+      <c r="AX2" s="2">
         <v>48</v>
       </c>
-      <c r="AY2" s="3">
+      <c r="AY2" s="2">
         <v>49</v>
       </c>
-      <c r="AZ2" s="3">
+      <c r="AZ2" s="2">
         <v>50</v>
       </c>
-      <c r="BA2" s="3">
+      <c r="BA2" s="2">
         <v>51</v>
       </c>
-      <c r="BB2" s="3">
+      <c r="BB2" s="2">
         <v>52</v>
       </c>
-      <c r="BC2" s="3">
+      <c r="BC2" s="2">
         <v>53</v>
       </c>
-      <c r="BD2" s="3">
+      <c r="BD2" s="2">
         <v>54</v>
       </c>
-      <c r="BE2" s="3">
+      <c r="BE2" s="2">
         <v>55</v>
       </c>
-      <c r="BF2" s="3">
+      <c r="BF2" s="2">
         <v>56</v>
       </c>
-      <c r="BG2" s="3">
+      <c r="BG2" s="2">
         <v>0</v>
       </c>
-      <c r="BH2" s="3">
+      <c r="BH2" s="2">
         <v>1</v>
       </c>
-      <c r="BI2" s="3">
+      <c r="BI2" s="2">
         <v>2</v>
       </c>
-      <c r="BJ2" s="3">
+      <c r="BJ2" s="2">
         <v>3</v>
       </c>
-      <c r="BK2" s="3">
+      <c r="BK2" s="2">
         <v>4</v>
       </c>
-      <c r="BL2" s="3">
+      <c r="BL2" s="2">
         <v>5</v>
       </c>
-      <c r="BM2" s="3">
+      <c r="BM2" s="2">
         <v>6</v>
       </c>
-      <c r="BN2" s="3">
+      <c r="BN2" s="2">
         <v>7</v>
       </c>
-      <c r="BO2" s="3">
+      <c r="BO2" s="2">
         <v>8</v>
       </c>
-      <c r="BP2" s="3">
+      <c r="BP2" s="2">
         <v>9</v>
       </c>
-      <c r="BQ2" s="3">
+      <c r="BQ2" s="2">
         <v>10</v>
       </c>
-      <c r="BR2" s="3">
+      <c r="BR2" s="2">
         <v>11</v>
       </c>
-      <c r="BS2" s="3">
+      <c r="BS2" s="2">
         <v>12</v>
       </c>
-      <c r="BT2" s="3">
+      <c r="BT2" s="2">
         <v>13</v>
       </c>
-      <c r="BU2" s="3">
+      <c r="BU2" s="2">
         <v>14</v>
       </c>
-      <c r="BV2" s="3">
+      <c r="BV2" s="2">
         <v>15</v>
       </c>
-      <c r="BW2" s="3">
+      <c r="BW2" s="2">
         <v>16</v>
       </c>
-      <c r="BX2" s="3">
+      <c r="BX2" s="2">
         <v>17</v>
       </c>
-      <c r="BY2" s="3">
+      <c r="BY2" s="2">
         <v>18</v>
       </c>
-      <c r="BZ2" s="3">
+      <c r="BZ2" s="2">
         <v>19</v>
       </c>
-      <c r="CA2" s="3">
+      <c r="CA2" s="2">
         <v>20</v>
       </c>
-      <c r="CB2" s="3">
+      <c r="CB2" s="2">
         <v>21</v>
       </c>
-      <c r="CC2" s="3">
+      <c r="CC2" s="2">
         <v>22</v>
       </c>
-      <c r="CD2" s="3">
+      <c r="CD2" s="2">
         <v>23</v>
       </c>
-      <c r="CE2" s="3">
+      <c r="CE2" s="2">
         <v>24</v>
       </c>
-      <c r="CF2" s="3">
+      <c r="CF2" s="2">
         <v>25</v>
       </c>
-      <c r="CG2" s="3">
+      <c r="CG2" s="2">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>0</v>
       </c>
       <c r="B3" s="1"/>
@@ -1727,7 +1721,7 @@
       </c>
     </row>
     <row r="4" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
@@ -1786,7 +1780,7 @@
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
       <c r="BE4" s="1"/>
-      <c r="BF4" t="s">
+      <c r="BF4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="BG4" s="1"/>
@@ -1818,7 +1812,7 @@
       <c r="CG4" s="1"/>
     </row>
     <row r="5" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
@@ -1877,7 +1871,7 @@
       <c r="BC5" s="1"/>
       <c r="BD5" s="1"/>
       <c r="BE5" s="1"/>
-      <c r="BF5" t="s">
+      <c r="BF5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="BG5" s="1"/>
@@ -1909,7 +1903,7 @@
       <c r="CG5" s="1"/>
     </row>
     <row r="6" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1972,7 +1966,7 @@
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
       <c r="BE6" s="1"/>
-      <c r="BF6" t="s">
+      <c r="BF6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="BG6" s="1"/>
@@ -2004,7 +1998,7 @@
       <c r="CG6" s="1"/>
     </row>
     <row r="7" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2067,7 +2061,7 @@
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
       <c r="BE7" s="1"/>
-      <c r="BF7" t="s">
+      <c r="BF7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="BG7" s="1"/>
@@ -2099,7 +2093,7 @@
       <c r="CG7" s="1"/>
     </row>
     <row r="8" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2162,7 +2156,7 @@
       <c r="BC8" s="1"/>
       <c r="BD8" s="1"/>
       <c r="BE8" s="1"/>
-      <c r="BF8" t="s">
+      <c r="BF8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="BG8" s="1"/>
@@ -2194,14 +2188,14 @@
       <c r="CG8" s="1"/>
     </row>
     <row r="9" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2257,7 +2251,7 @@
       <c r="BC9" s="1"/>
       <c r="BD9" s="1"/>
       <c r="BE9" s="1"/>
-      <c r="BF9" t="s">
+      <c r="BF9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="BG9" s="1"/>
@@ -2289,7 +2283,7 @@
       <c r="CG9" s="1"/>
     </row>
     <row r="10" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2352,7 +2346,7 @@
       <c r="BC10" s="1"/>
       <c r="BD10" s="1"/>
       <c r="BE10" s="1"/>
-      <c r="BF10" t="s">
+      <c r="BF10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="BG10" s="1"/>
@@ -2384,7 +2378,7 @@
       <c r="CG10" s="1"/>
     </row>
     <row r="11" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2447,7 +2441,7 @@
       <c r="BC11" s="1"/>
       <c r="BD11" s="1"/>
       <c r="BE11" s="1"/>
-      <c r="BF11" t="s">
+      <c r="BF11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="BG11" s="1"/>
@@ -2479,7 +2473,7 @@
       <c r="CG11" s="1"/>
     </row>
     <row r="12" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2544,7 +2538,7 @@
       <c r="BC12" s="1"/>
       <c r="BD12" s="1"/>
       <c r="BE12" s="1"/>
-      <c r="BF12" t="s">
+      <c r="BF12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="BG12" s="1"/>
@@ -2576,7 +2570,7 @@
       <c r="CG12" s="1"/>
     </row>
     <row r="13" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2639,7 +2633,7 @@
       <c r="BC13" s="1"/>
       <c r="BD13" s="1"/>
       <c r="BE13" s="1"/>
-      <c r="BF13" t="s">
+      <c r="BF13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="BG13" s="1"/>
@@ -2671,7 +2665,7 @@
       <c r="CG13" s="1"/>
     </row>
     <row r="14" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2743,7 +2737,9 @@
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
       <c r="AP14" s="1"/>
-      <c r="AQ14" s="1"/>
+      <c r="AQ14" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="AR14" s="1" t="s">
         <v>37</v>
       </c>
@@ -2778,7 +2774,7 @@
       <c r="BE14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BF14" t="s">
+      <c r="BF14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="BG14" s="1"/>
@@ -2814,7 +2810,7 @@
       <c r="CG14" s="1"/>
     </row>
     <row r="15" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2955,7 +2951,7 @@
       <c r="BE15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BF15" t="s">
+      <c r="BF15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="BG15" s="1"/>
@@ -2989,7 +2985,7 @@
       <c r="CG15" s="1"/>
     </row>
     <row r="16" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3104,7 +3100,7 @@
       <c r="BE16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BF16" t="s">
+      <c r="BF16" s="1" t="s">
         <v>60</v>
       </c>
       <c r="BG16" s="1"/>
@@ -3136,7 +3132,7 @@
       <c r="CG16" s="1"/>
     </row>
     <row r="17" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3251,7 +3247,7 @@
       <c r="BE17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BF17" t="s">
+      <c r="BF17" s="1" t="s">
         <v>62</v>
       </c>
       <c r="BG17" s="1"/>
@@ -3282,8 +3278,8 @@
       <c r="CF17" s="1"/>
       <c r="CG17" s="1"/>
     </row>
-    <row r="18" spans="1:85" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3409,7 +3405,7 @@
         <v>63</v>
       </c>
       <c r="AZ18" s="1" t="s">
-        <v>244</v>
+        <v>63</v>
       </c>
       <c r="BA18" s="1" t="s">
         <v>63</v>
@@ -3424,7 +3420,7 @@
       <c r="BE18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BF18" t="s">
+      <c r="BF18" s="1" t="s">
         <v>63</v>
       </c>
       <c r="BG18" s="1"/>
@@ -3456,7 +3452,7 @@
       <c r="CG18" s="1"/>
     </row>
     <row r="19" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3573,7 +3569,7 @@
       <c r="BE19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BF19" t="s">
+      <c r="BF19" s="1" t="s">
         <v>64</v>
       </c>
       <c r="BG19" s="1"/>
@@ -3605,7 +3601,7 @@
       <c r="CG19" s="1"/>
     </row>
     <row r="20" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3720,7 +3716,7 @@
       <c r="BE20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BF20" t="s">
+      <c r="BF20" s="1" t="s">
         <v>66</v>
       </c>
       <c r="BG20" s="1"/>
@@ -3752,7 +3748,7 @@
       <c r="CG20" s="1"/>
     </row>
     <row r="21" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3821,7 +3817,7 @@
       </c>
       <c r="BD21" s="1"/>
       <c r="BE21" s="1"/>
-      <c r="BF21" t="s">
+      <c r="BF21" s="1" t="s">
         <v>67</v>
       </c>
       <c r="BG21" s="1"/>
@@ -3853,7 +3849,7 @@
       <c r="CG21" s="1"/>
     </row>
     <row r="22" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -4000,7 +3996,7 @@
       <c r="BE22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BF22" t="s">
+      <c r="BF22" s="1" t="s">
         <v>68</v>
       </c>
       <c r="BG22" s="1"/>
@@ -4034,7 +4030,7 @@
       <c r="CG22" s="1"/>
     </row>
     <row r="23" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -4181,7 +4177,7 @@
       <c r="BE23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BF23" t="s">
+      <c r="BF23" s="1" t="s">
         <v>69</v>
       </c>
       <c r="BG23" s="1"/>
@@ -4219,7 +4215,7 @@
       <c r="CG23" s="1"/>
     </row>
     <row r="24" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>21</v>
       </c>
       <c r="B24" s="1"/>
@@ -4286,6 +4282,7 @@
       <c r="BC24" s="1"/>
       <c r="BD24" s="1"/>
       <c r="BE24" s="1"/>
+      <c r="BF24" s="1"/>
       <c r="BG24" s="1"/>
       <c r="BH24" s="1"/>
       <c r="BI24" s="1"/>
@@ -4331,7 +4328,7 @@
       <c r="CG24" s="1"/>
     </row>
     <row r="25" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>22</v>
       </c>
       <c r="B25" s="1"/>
@@ -4398,6 +4395,7 @@
       <c r="BC25" s="1"/>
       <c r="BD25" s="1"/>
       <c r="BE25" s="1"/>
+      <c r="BF25" s="1"/>
       <c r="BG25" s="1"/>
       <c r="BH25" s="1"/>
       <c r="BI25" s="1"/>
@@ -4443,7 +4441,7 @@
       <c r="CG25" s="1"/>
     </row>
     <row r="26" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>23</v>
       </c>
       <c r="B26" s="1"/>
@@ -4504,6 +4502,7 @@
       <c r="BC26" s="1"/>
       <c r="BD26" s="1"/>
       <c r="BE26" s="1"/>
+      <c r="BF26" s="1"/>
       <c r="BG26" s="1"/>
       <c r="BH26" s="1"/>
       <c r="BI26" s="1"/>
@@ -4535,7 +4534,7 @@
       <c r="CG26" s="1"/>
     </row>
     <row r="27" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>24</v>
       </c>
       <c r="B27" s="1"/>
@@ -4596,6 +4595,7 @@
       <c r="BC27" s="1"/>
       <c r="BD27" s="1"/>
       <c r="BE27" s="1"/>
+      <c r="BF27" s="1"/>
       <c r="BG27" s="1"/>
       <c r="BH27" s="1"/>
       <c r="BI27" s="1"/>
@@ -4625,7 +4625,7 @@
       <c r="CG27" s="1"/>
     </row>
     <row r="28" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>25</v>
       </c>
       <c r="B28" s="1"/>
@@ -4686,6 +4686,7 @@
       <c r="BC28" s="1"/>
       <c r="BD28" s="1"/>
       <c r="BE28" s="1"/>
+      <c r="BF28" s="1"/>
       <c r="BG28" s="1"/>
       <c r="BH28" s="1"/>
       <c r="BI28" s="1"/>
@@ -4715,7 +4716,7 @@
       <c r="CG28" s="1"/>
     </row>
     <row r="29" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>26</v>
       </c>
       <c r="B29" s="1"/>
@@ -4776,6 +4777,7 @@
       <c r="BC29" s="1"/>
       <c r="BD29" s="1"/>
       <c r="BE29" s="1"/>
+      <c r="BF29" s="1"/>
       <c r="BG29" s="1"/>
       <c r="BH29" s="1"/>
       <c r="BI29" s="1"/>
@@ -4805,7 +4807,7 @@
       <c r="CG29" s="1"/>
     </row>
     <row r="30" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>27</v>
       </c>
       <c r="B30" s="1"/>
@@ -4866,6 +4868,7 @@
       <c r="BC30" s="1"/>
       <c r="BD30" s="1"/>
       <c r="BE30" s="1"/>
+      <c r="BF30" s="1"/>
       <c r="BG30" s="1"/>
       <c r="BH30" s="1"/>
       <c r="BI30" s="1"/>
@@ -4897,7 +4900,7 @@
       <c r="CG30" s="1"/>
     </row>
     <row r="31" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>28</v>
       </c>
       <c r="B31" s="1"/>
@@ -4970,6 +4973,7 @@
       <c r="BC31" s="1"/>
       <c r="BD31" s="1"/>
       <c r="BE31" s="1"/>
+      <c r="BF31" s="1"/>
       <c r="BG31" s="1"/>
       <c r="BH31" s="1"/>
       <c r="BI31" s="1"/>
@@ -5017,7 +5021,7 @@
       </c>
     </row>
     <row r="32" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>29</v>
       </c>
       <c r="B32" s="1"/>
@@ -5090,6 +5094,7 @@
       <c r="BC32" s="1"/>
       <c r="BD32" s="1"/>
       <c r="BE32" s="1"/>
+      <c r="BF32" s="1"/>
       <c r="BG32" s="1"/>
       <c r="BH32" s="1"/>
       <c r="BI32" s="1"/>
@@ -5137,7 +5142,7 @@
       </c>
     </row>
     <row r="33" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -5226,7 +5231,7 @@
       <c r="BC33" s="1"/>
       <c r="BD33" s="1"/>
       <c r="BE33" s="1"/>
-      <c r="BF33" t="s">
+      <c r="BF33" s="1" t="s">
         <v>75</v>
       </c>
       <c r="BG33" s="1"/>
@@ -5292,7 +5297,7 @@
       </c>
     </row>
     <row r="34" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>31</v>
       </c>
       <c r="B34" s="1"/>
@@ -5373,6 +5378,7 @@
       <c r="BC34" s="1"/>
       <c r="BD34" s="1"/>
       <c r="BE34" s="1"/>
+      <c r="BF34" s="1"/>
       <c r="BG34" s="1"/>
       <c r="BH34" s="1">
         <v>95</v>
@@ -5436,7 +5442,7 @@
       </c>
     </row>
     <row r="35" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>32</v>
       </c>
       <c r="B35" s="1"/>
@@ -5507,6 +5513,7 @@
       <c r="BC35" s="1"/>
       <c r="BD35" s="1"/>
       <c r="BE35" s="1"/>
+      <c r="BF35" s="1"/>
       <c r="BG35" s="1"/>
       <c r="BH35" s="1"/>
       <c r="BI35" s="1"/>
@@ -5542,7 +5549,7 @@
       </c>
     </row>
     <row r="36" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>33</v>
       </c>
       <c r="B36" s="1"/>
@@ -5609,6 +5616,7 @@
       <c r="BC36" s="1"/>
       <c r="BD36" s="1"/>
       <c r="BE36" s="1"/>
+      <c r="BF36" s="1"/>
       <c r="BG36" s="1"/>
       <c r="BH36" s="1"/>
       <c r="BI36" s="1"/>
@@ -5654,7 +5662,7 @@
       <c r="CG36" s="1"/>
     </row>
     <row r="37" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>34</v>
       </c>
       <c r="B37" s="1"/>
@@ -5721,6 +5729,7 @@
       <c r="BC37" s="1"/>
       <c r="BD37" s="1"/>
       <c r="BE37" s="1"/>
+      <c r="BF37" s="1"/>
       <c r="BG37" s="1"/>
       <c r="BH37" s="1"/>
       <c r="BI37" s="1"/>
@@ -5750,7 +5759,7 @@
       <c r="CG37" s="1"/>
     </row>
     <row r="38" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>35</v>
       </c>
       <c r="B38" s="1"/>
@@ -5817,6 +5826,7 @@
       <c r="BC38" s="1"/>
       <c r="BD38" s="1"/>
       <c r="BE38" s="1"/>
+      <c r="BF38" s="1"/>
       <c r="BG38" s="1"/>
       <c r="BH38" s="1"/>
       <c r="BI38" s="1"/>
@@ -5846,7 +5856,7 @@
       <c r="CG38" s="1"/>
     </row>
     <row r="39" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>36</v>
       </c>
       <c r="B39" s="1"/>
@@ -5913,6 +5923,7 @@
       <c r="BC39" s="1"/>
       <c r="BD39" s="1"/>
       <c r="BE39" s="1"/>
+      <c r="BF39" s="1"/>
       <c r="BG39" s="1"/>
       <c r="BH39" s="1"/>
       <c r="BI39" s="1"/>
@@ -5942,7 +5953,7 @@
       <c r="CG39" s="1"/>
     </row>
     <row r="40" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>37</v>
       </c>
       <c r="B40" s="1"/>
@@ -6009,6 +6020,7 @@
       <c r="BC40" s="1"/>
       <c r="BD40" s="1"/>
       <c r="BE40" s="1"/>
+      <c r="BF40" s="1"/>
       <c r="BG40" s="1"/>
       <c r="BH40" s="1"/>
       <c r="BI40" s="1"/>
@@ -6038,7 +6050,7 @@
       <c r="CG40" s="1"/>
     </row>
     <row r="41" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>38</v>
       </c>
       <c r="B41" s="1"/>
@@ -6105,6 +6117,7 @@
       <c r="BC41" s="1"/>
       <c r="BD41" s="1"/>
       <c r="BE41" s="1"/>
+      <c r="BF41" s="1"/>
       <c r="BG41" s="1"/>
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
@@ -6134,7 +6147,7 @@
       <c r="CG41" s="1"/>
     </row>
     <row r="42" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>39</v>
       </c>
       <c r="B42" s="1"/>
@@ -6201,6 +6214,7 @@
       <c r="BC42" s="1"/>
       <c r="BD42" s="1"/>
       <c r="BE42" s="1"/>
+      <c r="BF42" s="1"/>
       <c r="BG42" s="1"/>
       <c r="BH42" s="1"/>
       <c r="BI42" s="1"/>
@@ -6230,7 +6244,7 @@
       <c r="CG42" s="1"/>
     </row>
     <row r="43" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="A43" s="4">
         <v>40</v>
       </c>
       <c r="B43" s="1"/>
@@ -6297,6 +6311,7 @@
       <c r="BC43" s="1"/>
       <c r="BD43" s="1"/>
       <c r="BE43" s="1"/>
+      <c r="BF43" s="1"/>
       <c r="BG43" s="1"/>
       <c r="BH43" s="1"/>
       <c r="BI43" s="1"/>
@@ -6326,7 +6341,7 @@
       <c r="CG43" s="1"/>
     </row>
     <row r="44" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>41</v>
       </c>
       <c r="B44" s="1"/>
@@ -6393,6 +6408,7 @@
       <c r="BC44" s="1"/>
       <c r="BD44" s="1"/>
       <c r="BE44" s="1"/>
+      <c r="BF44" s="1"/>
       <c r="BG44" s="1"/>
       <c r="BH44" s="1"/>
       <c r="BI44" s="1"/>
@@ -6422,7 +6438,7 @@
       <c r="CG44" s="1"/>
     </row>
     <row r="45" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+      <c r="A45" s="4">
         <v>42</v>
       </c>
       <c r="B45" s="1"/>
@@ -6489,6 +6505,7 @@
       <c r="BC45" s="1"/>
       <c r="BD45" s="1"/>
       <c r="BE45" s="1"/>
+      <c r="BF45" s="1"/>
       <c r="BG45" s="1"/>
       <c r="BH45" s="1"/>
       <c r="BI45" s="1"/>
@@ -6518,7 +6535,7 @@
       <c r="CG45" s="1"/>
     </row>
     <row r="46" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="4">
         <v>43</v>
       </c>
       <c r="B46" s="1"/>
@@ -6585,6 +6602,7 @@
       <c r="BC46" s="1"/>
       <c r="BD46" s="1"/>
       <c r="BE46" s="1"/>
+      <c r="BF46" s="1"/>
       <c r="BG46" s="1"/>
       <c r="BH46" s="1"/>
       <c r="BI46" s="1"/>
@@ -6614,7 +6632,7 @@
       <c r="CG46" s="1"/>
     </row>
     <row r="47" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="A47" s="4">
         <v>44</v>
       </c>
       <c r="B47" s="1"/>
@@ -6681,6 +6699,7 @@
       <c r="BC47" s="1"/>
       <c r="BD47" s="1"/>
       <c r="BE47" s="1"/>
+      <c r="BF47" s="1"/>
       <c r="BG47" s="1"/>
       <c r="BH47" s="1"/>
       <c r="BI47" s="1"/>
@@ -6710,7 +6729,7 @@
       <c r="CG47" s="1"/>
     </row>
     <row r="48" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="A48" s="4">
         <v>45</v>
       </c>
       <c r="B48" s="1"/>
@@ -6777,6 +6796,7 @@
       <c r="BC48" s="1"/>
       <c r="BD48" s="1"/>
       <c r="BE48" s="1"/>
+      <c r="BF48" s="1"/>
       <c r="BG48" s="1"/>
       <c r="BH48" s="1"/>
       <c r="BI48" s="1"/>
@@ -6806,7 +6826,7 @@
       <c r="CG48" s="1"/>
     </row>
     <row r="49" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+      <c r="A49" s="4">
         <v>46</v>
       </c>
       <c r="B49" s="1"/>
@@ -6873,6 +6893,7 @@
       <c r="BC49" s="1"/>
       <c r="BD49" s="1"/>
       <c r="BE49" s="1"/>
+      <c r="BF49" s="1"/>
       <c r="BG49" s="1"/>
       <c r="BH49" s="1"/>
       <c r="BI49" s="1"/>
@@ -6902,7 +6923,7 @@
       <c r="CG49" s="1"/>
     </row>
     <row r="50" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>47</v>
       </c>
       <c r="B50" s="1"/>
@@ -6969,6 +6990,7 @@
       <c r="BC50" s="1"/>
       <c r="BD50" s="1"/>
       <c r="BE50" s="1"/>
+      <c r="BF50" s="1"/>
       <c r="BG50" s="1"/>
       <c r="BH50" s="1"/>
       <c r="BI50" s="1"/>
@@ -6998,7 +7020,7 @@
       <c r="CG50" s="1"/>
     </row>
     <row r="51" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+      <c r="A51" s="4">
         <v>48</v>
       </c>
       <c r="B51" s="1"/>
@@ -7065,6 +7087,7 @@
       <c r="BC51" s="1"/>
       <c r="BD51" s="1"/>
       <c r="BE51" s="1"/>
+      <c r="BF51" s="1"/>
       <c r="BG51" s="1"/>
       <c r="BH51" s="1"/>
       <c r="BI51" s="1"/>
@@ -7094,7 +7117,7 @@
       <c r="CG51" s="1"/>
     </row>
     <row r="52" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+      <c r="A52" s="4">
         <v>49</v>
       </c>
       <c r="B52" s="1"/>
@@ -7161,6 +7184,7 @@
       <c r="BC52" s="1"/>
       <c r="BD52" s="1"/>
       <c r="BE52" s="1"/>
+      <c r="BF52" s="1"/>
       <c r="BG52" s="1"/>
       <c r="BH52" s="1"/>
       <c r="BI52" s="1"/>
@@ -7190,7 +7214,7 @@
       <c r="CG52" s="1"/>
     </row>
     <row r="53" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
+      <c r="A53" s="4">
         <v>50</v>
       </c>
       <c r="B53" s="1"/>
@@ -7257,6 +7281,7 @@
       <c r="BC53" s="1"/>
       <c r="BD53" s="1"/>
       <c r="BE53" s="1"/>
+      <c r="BF53" s="1"/>
       <c r="BG53" s="1"/>
       <c r="BH53" s="1"/>
       <c r="BI53" s="1"/>
@@ -7286,7 +7311,7 @@
       <c r="CG53" s="1"/>
     </row>
     <row r="54" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
+      <c r="A54" s="4">
         <v>51</v>
       </c>
       <c r="B54" s="1"/>
@@ -7353,6 +7378,7 @@
       <c r="BC54" s="1"/>
       <c r="BD54" s="1"/>
       <c r="BE54" s="1"/>
+      <c r="BF54" s="1"/>
       <c r="BG54" s="1"/>
       <c r="BH54" s="1"/>
       <c r="BI54" s="1"/>
@@ -7382,7 +7408,7 @@
       <c r="CG54" s="1"/>
     </row>
     <row r="55" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
+      <c r="A55" s="4">
         <v>52</v>
       </c>
       <c r="B55" s="1"/>
@@ -7449,6 +7475,7 @@
       <c r="BC55" s="1"/>
       <c r="BD55" s="1"/>
       <c r="BE55" s="1"/>
+      <c r="BF55" s="1"/>
       <c r="BG55" s="1"/>
       <c r="BH55" s="1"/>
       <c r="BI55" s="1"/>
@@ -7478,7 +7505,7 @@
       <c r="CG55" s="1"/>
     </row>
     <row r="56" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
+      <c r="A56" s="4">
         <v>53</v>
       </c>
       <c r="B56" s="1"/>
@@ -7545,6 +7572,7 @@
       <c r="BC56" s="1"/>
       <c r="BD56" s="1"/>
       <c r="BE56" s="1"/>
+      <c r="BF56" s="1"/>
       <c r="BG56" s="1"/>
       <c r="BH56" s="1"/>
       <c r="BI56" s="1"/>
@@ -7590,7 +7618,7 @@
       <c r="CG56" s="1"/>
     </row>
     <row r="57" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+      <c r="A57" s="4">
         <v>54</v>
       </c>
       <c r="B57" s="1"/>
@@ -7657,6 +7685,7 @@
       <c r="BC57" s="1"/>
       <c r="BD57" s="1"/>
       <c r="BE57" s="1"/>
+      <c r="BF57" s="1"/>
       <c r="BG57" s="1"/>
       <c r="BH57" s="1"/>
       <c r="BI57" s="1"/>
@@ -7686,7 +7715,7 @@
       <c r="CG57" s="1"/>
     </row>
     <row r="58" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
+      <c r="A58" s="4">
         <v>55</v>
       </c>
       <c r="B58" s="1"/>
@@ -7753,6 +7782,7 @@
       <c r="BC58" s="1"/>
       <c r="BD58" s="1"/>
       <c r="BE58" s="1"/>
+      <c r="BF58" s="1"/>
       <c r="BG58" s="1"/>
       <c r="BH58" s="1"/>
       <c r="BI58" s="1"/>
@@ -7782,7 +7812,7 @@
       <c r="CG58" s="1"/>
     </row>
     <row r="59" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+      <c r="A59" s="4">
         <v>56</v>
       </c>
       <c r="B59" s="1"/>
@@ -7849,6 +7879,7 @@
       <c r="BC59" s="1"/>
       <c r="BD59" s="1"/>
       <c r="BE59" s="1"/>
+      <c r="BF59" s="1"/>
       <c r="BG59" s="1"/>
       <c r="BH59" s="1"/>
       <c r="BI59" s="1"/>
@@ -7878,7 +7909,7 @@
       <c r="CG59" s="1"/>
     </row>
     <row r="60" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+      <c r="A60" s="4">
         <v>57</v>
       </c>
       <c r="B60" s="1"/>
@@ -7941,6 +7972,7 @@
       <c r="BC60" s="1"/>
       <c r="BD60" s="1"/>
       <c r="BE60" s="1"/>
+      <c r="BF60" s="1"/>
       <c r="BG60" s="1"/>
       <c r="BH60" s="1"/>
       <c r="BI60" s="1"/>
@@ -7982,7 +8014,7 @@
       <c r="CG60" s="1"/>
     </row>
     <row r="61" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="A61" s="4">
         <v>58</v>
       </c>
       <c r="B61" s="1"/>
@@ -8045,6 +8077,7 @@
       <c r="BC61" s="1"/>
       <c r="BD61" s="1"/>
       <c r="BE61" s="1"/>
+      <c r="BF61" s="1"/>
       <c r="BG61" s="1"/>
       <c r="BH61" s="1"/>
       <c r="BI61" s="1"/>
@@ -8074,7 +8107,7 @@
       <c r="CG61" s="1"/>
     </row>
     <row r="62" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
+      <c r="A62" s="4">
         <v>59</v>
       </c>
       <c r="B62" s="1"/>
@@ -8137,6 +8170,7 @@
       <c r="BC62" s="1"/>
       <c r="BD62" s="1"/>
       <c r="BE62" s="1"/>
+      <c r="BF62" s="1"/>
       <c r="BG62" s="1"/>
       <c r="BH62" s="1"/>
       <c r="BI62" s="1"/>
@@ -8166,7 +8200,7 @@
       <c r="CG62" s="1"/>
     </row>
     <row r="63" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
+      <c r="A63" s="4">
         <v>60</v>
       </c>
       <c r="B63" s="1"/>
@@ -8229,6 +8263,7 @@
       <c r="BC63" s="1"/>
       <c r="BD63" s="1"/>
       <c r="BE63" s="1"/>
+      <c r="BF63" s="1"/>
       <c r="BG63" s="1"/>
       <c r="BH63" s="1"/>
       <c r="BI63" s="1"/>
@@ -8258,7 +8293,7 @@
       <c r="CG63" s="1"/>
     </row>
     <row r="64" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
+      <c r="A64" s="4">
         <v>61</v>
       </c>
       <c r="B64" s="1"/>
@@ -8321,6 +8356,7 @@
       <c r="BC64" s="1"/>
       <c r="BD64" s="1"/>
       <c r="BE64" s="1"/>
+      <c r="BF64" s="1"/>
       <c r="BG64" s="1"/>
       <c r="BH64" s="1"/>
       <c r="BI64" s="1"/>
@@ -8350,7 +8386,7 @@
       <c r="CG64" s="1"/>
     </row>
     <row r="65" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="4">
         <v>62</v>
       </c>
       <c r="B65" s="1"/>
@@ -8413,6 +8449,7 @@
       <c r="BC65" s="1"/>
       <c r="BD65" s="1"/>
       <c r="BE65" s="1"/>
+      <c r="BF65" s="1"/>
       <c r="BG65" s="1"/>
       <c r="BH65" s="1"/>
       <c r="BI65" s="1"/>
@@ -8442,7 +8479,7 @@
       <c r="CG65" s="1"/>
     </row>
     <row r="66" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
+      <c r="A66" s="4">
         <v>63</v>
       </c>
       <c r="B66" s="1"/>
@@ -8505,6 +8542,7 @@
       <c r="BC66" s="1"/>
       <c r="BD66" s="1"/>
       <c r="BE66" s="1"/>
+      <c r="BF66" s="1"/>
       <c r="BG66" s="1"/>
       <c r="BH66" s="1"/>
       <c r="BI66" s="1"/>
@@ -8534,7 +8572,7 @@
       <c r="CG66" s="1"/>
     </row>
     <row r="67" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+      <c r="A67" s="4">
         <v>64</v>
       </c>
       <c r="B67" s="1"/>
@@ -8597,6 +8635,7 @@
       <c r="BC67" s="1"/>
       <c r="BD67" s="1"/>
       <c r="BE67" s="1"/>
+      <c r="BF67" s="1"/>
       <c r="BG67" s="1"/>
       <c r="BH67" s="1"/>
       <c r="BI67" s="1"/>
@@ -8626,7 +8665,7 @@
       <c r="CG67" s="1"/>
     </row>
     <row r="68" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
+      <c r="A68" s="4">
         <v>65</v>
       </c>
       <c r="B68" s="1"/>
@@ -8689,6 +8728,7 @@
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="1"/>
+      <c r="BF68" s="1"/>
       <c r="BG68" s="1"/>
       <c r="BH68" s="1"/>
       <c r="BI68" s="1"/>
@@ -8718,7 +8758,7 @@
       <c r="CG68" s="1"/>
     </row>
     <row r="69" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+      <c r="A69" s="4">
         <v>66</v>
       </c>
       <c r="B69" s="1"/>
@@ -8781,6 +8821,7 @@
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="1"/>
+      <c r="BF69" s="1"/>
       <c r="BG69" s="1"/>
       <c r="BH69" s="1"/>
       <c r="BI69" s="1"/>
@@ -8810,7 +8851,7 @@
       <c r="CG69" s="1"/>
     </row>
     <row r="70" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
+      <c r="A70" s="4">
         <v>67</v>
       </c>
       <c r="B70" s="1"/>
@@ -8873,6 +8914,7 @@
       <c r="BC70" s="1"/>
       <c r="BD70" s="1"/>
       <c r="BE70" s="1"/>
+      <c r="BF70" s="1"/>
       <c r="BG70" s="1"/>
       <c r="BH70" s="1"/>
       <c r="BI70" s="1"/>
@@ -8902,7 +8944,7 @@
       <c r="CG70" s="1"/>
     </row>
     <row r="71" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
+      <c r="A71" s="4">
         <v>68</v>
       </c>
       <c r="B71" s="1"/>
@@ -8965,6 +9007,7 @@
       <c r="BC71" s="1"/>
       <c r="BD71" s="1"/>
       <c r="BE71" s="1"/>
+      <c r="BF71" s="1"/>
       <c r="BG71" s="1"/>
       <c r="BH71" s="1"/>
       <c r="BI71" s="1"/>
@@ -8994,7 +9037,7 @@
       <c r="CG71" s="1"/>
     </row>
     <row r="72" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
+      <c r="A72" s="4">
         <v>69</v>
       </c>
       <c r="B72" s="1"/>
@@ -9057,6 +9100,7 @@
       <c r="BC72" s="1"/>
       <c r="BD72" s="1"/>
       <c r="BE72" s="1"/>
+      <c r="BF72" s="1"/>
       <c r="BG72" s="1"/>
       <c r="BH72" s="1"/>
       <c r="BI72" s="1"/>
@@ -9086,7 +9130,7 @@
       <c r="CG72" s="1"/>
     </row>
     <row r="73" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
+      <c r="A73" s="4">
         <v>70</v>
       </c>
       <c r="B73" s="1"/>
@@ -9149,6 +9193,7 @@
       <c r="BC73" s="1"/>
       <c r="BD73" s="1"/>
       <c r="BE73" s="1"/>
+      <c r="BF73" s="1"/>
       <c r="BG73" s="1"/>
       <c r="BH73" s="1"/>
       <c r="BI73" s="1"/>
@@ -9178,7 +9223,7 @@
       <c r="CG73" s="1"/>
     </row>
     <row r="74" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
+      <c r="A74" s="4">
         <v>71</v>
       </c>
       <c r="B74" s="1"/>
@@ -9245,6 +9290,7 @@
       <c r="BC74" s="1"/>
       <c r="BD74" s="1"/>
       <c r="BE74" s="1"/>
+      <c r="BF74" s="1"/>
       <c r="BG74" s="1"/>
       <c r="BH74" s="1"/>
       <c r="BI74" s="1"/>
@@ -9288,7 +9334,7 @@
       <c r="CG74" s="1"/>
     </row>
     <row r="75" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
+      <c r="A75" s="4">
         <v>72</v>
       </c>
       <c r="B75" s="1"/>
@@ -9359,6 +9405,7 @@
       <c r="BC75" s="1"/>
       <c r="BD75" s="1"/>
       <c r="BE75" s="1"/>
+      <c r="BF75" s="1"/>
       <c r="BG75" s="1"/>
       <c r="BH75" s="1"/>
       <c r="BI75" s="1"/>
@@ -9394,7 +9441,7 @@
       </c>
     </row>
     <row r="76" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
+      <c r="A76" s="4">
         <v>73</v>
       </c>
       <c r="B76" s="1"/>
@@ -9455,6 +9502,7 @@
       <c r="BC76" s="1"/>
       <c r="BD76" s="1"/>
       <c r="BE76" s="1"/>
+      <c r="BF76" s="1"/>
       <c r="BG76" s="1"/>
       <c r="BH76" s="1"/>
       <c r="BI76" s="1"/>
@@ -9486,7 +9534,7 @@
       <c r="CG76" s="1"/>
     </row>
     <row r="77" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
+      <c r="A77" s="4">
         <v>74</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -9631,7 +9679,7 @@
       <c r="BE77" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BF77" t="s">
+      <c r="BF77" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BG77" s="1"/>
@@ -9663,7 +9711,7 @@
       <c r="CG77" s="1"/>
     </row>
     <row r="78" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
+      <c r="A78" s="4">
         <v>75</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -9806,7 +9854,7 @@
       <c r="BE78" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BF78" t="s">
+      <c r="BF78" s="1" t="s">
         <v>114</v>
       </c>
       <c r="BG78" s="1"/>
@@ -9838,7 +9886,7 @@
       <c r="CG78" s="1"/>
     </row>
     <row r="79" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
+      <c r="A79" s="4">
         <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -9981,7 +10029,7 @@
       <c r="BE79" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="BF79" t="s">
+      <c r="BF79" s="1" t="s">
         <v>115</v>
       </c>
       <c r="BG79" s="1"/>
@@ -10013,7 +10061,7 @@
       <c r="CG79" s="1"/>
     </row>
     <row r="80" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
+      <c r="A80" s="4">
         <v>77</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -10156,7 +10204,7 @@
       <c r="BE80" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="BF80" t="s">
+      <c r="BF80" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BG80" s="1"/>
@@ -10188,7 +10236,7 @@
       <c r="CG80" s="1"/>
     </row>
     <row r="81" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
+      <c r="A81" s="4">
         <v>78</v>
       </c>
       <c r="B81" s="1"/>
@@ -10269,6 +10317,7 @@
       <c r="BC81" s="1"/>
       <c r="BD81" s="1"/>
       <c r="BE81" s="1"/>
+      <c r="BF81" s="1"/>
       <c r="BG81" s="1"/>
       <c r="BH81" s="1"/>
       <c r="BI81" s="1"/>
@@ -10300,7 +10349,7 @@
       <c r="CG81" s="1"/>
     </row>
     <row r="82" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
+      <c r="A82" s="4">
         <v>79</v>
       </c>
       <c r="B82" s="1"/>
@@ -10361,6 +10410,7 @@
       <c r="BC82" s="1"/>
       <c r="BD82" s="1"/>
       <c r="BE82" s="1"/>
+      <c r="BF82" s="1"/>
       <c r="BG82" s="1"/>
       <c r="BH82" s="1"/>
       <c r="BI82" s="1"/>
@@ -10390,7 +10440,7 @@
       <c r="CG82" s="1"/>
     </row>
     <row r="83" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
+      <c r="A83" s="4">
         <v>80</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -10505,7 +10555,7 @@
       <c r="BE83" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BF83" t="s">
+      <c r="BF83" s="1" t="s">
         <v>46</v>
       </c>
       <c r="BG83" s="1"/>
@@ -10537,7 +10587,7 @@
       <c r="CG83" s="1"/>
     </row>
     <row r="84" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
+      <c r="A84" s="4">
         <v>81</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -10678,7 +10728,7 @@
       <c r="BE84" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BF84" t="s">
+      <c r="BF84" s="1" t="s">
         <v>63</v>
       </c>
       <c r="BG84" s="1"/>
@@ -10710,7 +10760,7 @@
       <c r="CG84" s="1"/>
     </row>
     <row r="85" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
+      <c r="A85" s="4">
         <v>82</v>
       </c>
       <c r="B85" s="1"/>
@@ -10777,6 +10827,7 @@
       <c r="BC85" s="1"/>
       <c r="BD85" s="1"/>
       <c r="BE85" s="1"/>
+      <c r="BF85" s="1"/>
       <c r="BG85" s="1"/>
       <c r="BH85" s="1"/>
       <c r="BI85" s="1"/>
@@ -10820,7 +10871,7 @@
       <c r="CG85" s="1"/>
     </row>
     <row r="86" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
+      <c r="A86" s="4">
         <v>83</v>
       </c>
       <c r="B86" s="1"/>
@@ -10887,6 +10938,7 @@
       <c r="BC86" s="1"/>
       <c r="BD86" s="1"/>
       <c r="BE86" s="1"/>
+      <c r="BF86" s="1"/>
       <c r="BG86" s="1"/>
       <c r="BH86" s="1"/>
       <c r="BI86" s="1"/>
@@ -10930,7 +10982,7 @@
       <c r="CG86" s="1"/>
     </row>
     <row r="87" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
+      <c r="A87" s="4">
         <v>84</v>
       </c>
       <c r="B87" s="1"/>
@@ -10991,6 +11043,7 @@
       <c r="BC87" s="1"/>
       <c r="BD87" s="1"/>
       <c r="BE87" s="1"/>
+      <c r="BF87" s="1"/>
       <c r="BG87" s="1"/>
       <c r="BH87" s="1"/>
       <c r="BI87" s="1"/>
@@ -11020,7 +11073,7 @@
       <c r="CG87" s="1"/>
     </row>
     <row r="88" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
+      <c r="A88" s="4">
         <v>85</v>
       </c>
       <c r="B88" s="1"/>
@@ -11081,6 +11134,7 @@
       <c r="BC88" s="1"/>
       <c r="BD88" s="1"/>
       <c r="BE88" s="1"/>
+      <c r="BF88" s="1"/>
       <c r="BG88" s="1"/>
       <c r="BH88" s="1"/>
       <c r="BI88" s="1"/>
@@ -11110,7 +11164,7 @@
       <c r="CG88" s="1"/>
     </row>
     <row r="89" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
+      <c r="A89" s="4">
         <v>86</v>
       </c>
       <c r="B89" s="1"/>
@@ -11177,6 +11231,7 @@
       <c r="BC89" s="1"/>
       <c r="BD89" s="1"/>
       <c r="BE89" s="1"/>
+      <c r="BF89" s="1"/>
       <c r="BG89" s="1"/>
       <c r="BH89" s="1"/>
       <c r="BI89" s="1"/>
@@ -11222,7 +11277,7 @@
       <c r="CG89" s="1"/>
     </row>
     <row r="90" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
+      <c r="A90" s="4">
         <v>87</v>
       </c>
       <c r="B90" s="1"/>
@@ -11289,10 +11344,13 @@
       <c r="BC90" s="1"/>
       <c r="BD90" s="1"/>
       <c r="BE90" s="1"/>
+      <c r="BF90" s="1"/>
       <c r="BG90" s="1"/>
       <c r="BH90" s="1"/>
       <c r="BI90" s="1"/>
-      <c r="BJ90" s="1"/>
+      <c r="BJ90" s="1">
+        <v>112</v>
+      </c>
       <c r="BK90" s="1"/>
       <c r="BL90" s="1"/>
       <c r="BM90" s="1"/>
@@ -11300,14 +11358,12 @@
       <c r="BO90" s="1"/>
       <c r="BP90" s="1"/>
       <c r="BQ90" s="1">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="BR90" s="1"/>
       <c r="BS90" s="1"/>
       <c r="BT90" s="1"/>
-      <c r="BU90" s="1">
-        <v>112</v>
-      </c>
+      <c r="BU90" s="1"/>
       <c r="BV90" s="1">
         <v>80</v>
       </c>
@@ -11334,7 +11390,7 @@
       <c r="CG90" s="1"/>
     </row>
     <row r="91" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
+      <c r="A91" s="4">
         <v>88</v>
       </c>
       <c r="B91" s="1"/>
@@ -11397,6 +11453,7 @@
       <c r="BC91" s="1"/>
       <c r="BD91" s="1"/>
       <c r="BE91" s="1"/>
+      <c r="BF91" s="1"/>
       <c r="BG91" s="1"/>
       <c r="BH91" s="1"/>
       <c r="BI91" s="1"/>
@@ -11432,7 +11489,7 @@
       <c r="CG91" s="1"/>
     </row>
     <row r="92" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
+      <c r="A92" s="4">
         <v>89</v>
       </c>
       <c r="B92" s="1"/>
@@ -11493,6 +11550,7 @@
       <c r="BC92" s="1"/>
       <c r="BD92" s="1"/>
       <c r="BE92" s="1"/>
+      <c r="BF92" s="1"/>
       <c r="BG92" s="1"/>
       <c r="BH92" s="1"/>
       <c r="BI92" s="1"/>
@@ -11522,7 +11580,7 @@
       <c r="CG92" s="1"/>
     </row>
     <row r="93" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
+      <c r="A93" s="4">
         <v>90</v>
       </c>
       <c r="B93" s="1"/>
@@ -11585,6 +11643,7 @@
       <c r="BC93" s="1"/>
       <c r="BD93" s="1"/>
       <c r="BE93" s="1"/>
+      <c r="BF93" s="1"/>
       <c r="BG93" s="1"/>
       <c r="BH93" s="1"/>
       <c r="BI93" s="1"/>
@@ -11614,7 +11673,7 @@
       <c r="CG93" s="1"/>
     </row>
     <row r="94" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
+      <c r="A94" s="4">
         <v>91</v>
       </c>
       <c r="B94" s="1"/>
@@ -11675,6 +11734,7 @@
       <c r="BC94" s="1"/>
       <c r="BD94" s="1"/>
       <c r="BE94" s="1"/>
+      <c r="BF94" s="1"/>
       <c r="BG94" s="1"/>
       <c r="BH94" s="1"/>
       <c r="BI94" s="1"/>
@@ -11704,7 +11764,7 @@
       <c r="CG94" s="1"/>
     </row>
     <row r="95" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
+      <c r="A95" s="4">
         <v>92</v>
       </c>
       <c r="B95" s="1"/>
@@ -11767,6 +11827,7 @@
       </c>
       <c r="BD95" s="1"/>
       <c r="BE95" s="1"/>
+      <c r="BF95" s="1"/>
       <c r="BG95" s="1"/>
       <c r="BH95" s="1"/>
       <c r="BI95" s="1"/>
@@ -11796,7 +11857,7 @@
       <c r="CG95" s="1"/>
     </row>
     <row r="96" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
+      <c r="A96" s="4">
         <v>93</v>
       </c>
       <c r="B96" s="1"/>
@@ -11857,6 +11918,7 @@
       </c>
       <c r="BD96" s="1"/>
       <c r="BE96" s="1"/>
+      <c r="BF96" s="1"/>
       <c r="BG96" s="1"/>
       <c r="BH96" s="1"/>
       <c r="BI96" s="1"/>
@@ -11886,7 +11948,7 @@
       <c r="CG96" s="1"/>
     </row>
     <row r="97" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
+      <c r="A97" s="4">
         <v>94</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -11953,7 +12015,7 @@
       <c r="BC97" s="1"/>
       <c r="BD97" s="1"/>
       <c r="BE97" s="1"/>
-      <c r="BF97" t="s">
+      <c r="BF97" s="1" t="s">
         <v>125</v>
       </c>
       <c r="BG97" s="1"/>
@@ -11985,7 +12047,7 @@
       <c r="CG97" s="1"/>
     </row>
     <row r="98" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
+      <c r="A98" s="4">
         <v>95</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -12052,7 +12114,7 @@
       <c r="BC98" s="1"/>
       <c r="BD98" s="1"/>
       <c r="BE98" s="1"/>
-      <c r="BF98" t="s">
+      <c r="BF98" s="1" t="s">
         <v>126</v>
       </c>
       <c r="BG98" s="1"/>
@@ -12084,7 +12146,7 @@
       <c r="CG98" s="1"/>
     </row>
     <row r="99" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
+      <c r="A99" s="4">
         <v>96</v>
       </c>
       <c r="B99" s="1" t="s">
@@ -12153,7 +12215,7 @@
       </c>
       <c r="BD99" s="1"/>
       <c r="BE99" s="1"/>
-      <c r="BF99" t="s">
+      <c r="BF99" s="1" t="s">
         <v>127</v>
       </c>
       <c r="BG99" s="1"/>
@@ -12185,7 +12247,7 @@
       <c r="CG99" s="1"/>
     </row>
     <row r="100" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A100" s="5">
+      <c r="A100" s="4">
         <v>97</v>
       </c>
       <c r="B100" s="1"/>
@@ -12246,6 +12308,7 @@
       <c r="BC100" s="1"/>
       <c r="BD100" s="1"/>
       <c r="BE100" s="1"/>
+      <c r="BF100" s="1"/>
       <c r="BG100" s="1"/>
       <c r="BH100" s="1"/>
       <c r="BI100" s="1"/>
@@ -12275,7 +12338,7 @@
       <c r="CG100" s="1"/>
     </row>
     <row r="101" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
+      <c r="A101" s="4">
         <v>98</v>
       </c>
       <c r="B101" s="1"/>
@@ -12346,6 +12409,7 @@
       <c r="BC101" s="1"/>
       <c r="BD101" s="1"/>
       <c r="BE101" s="1"/>
+      <c r="BF101" s="1"/>
       <c r="BG101" s="1"/>
       <c r="BH101" s="1"/>
       <c r="BI101" s="1"/>
@@ -12381,7 +12445,7 @@
       </c>
     </row>
     <row r="102" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A102" s="5">
+      <c r="A102" s="4">
         <v>99</v>
       </c>
       <c r="B102" s="1"/>
@@ -12452,6 +12516,7 @@
       <c r="BC102" s="1"/>
       <c r="BD102" s="1"/>
       <c r="BE102" s="1"/>
+      <c r="BF102" s="1"/>
       <c r="BG102" s="1"/>
       <c r="BH102" s="1"/>
       <c r="BI102" s="1"/>
@@ -12487,7 +12552,7 @@
       </c>
     </row>
     <row r="103" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
+      <c r="A103" s="4">
         <v>100</v>
       </c>
       <c r="B103" s="1" t="s">
@@ -12533,7 +12598,9 @@
       <c r="AN103" s="1"/>
       <c r="AO103" s="1"/>
       <c r="AP103" s="1"/>
-      <c r="AQ103" s="1"/>
+      <c r="AQ103" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="AR103" s="1"/>
       <c r="AS103" s="1"/>
       <c r="AT103" s="1"/>
@@ -12550,7 +12617,7 @@
       <c r="BC103" s="1"/>
       <c r="BD103" s="1"/>
       <c r="BE103" s="1"/>
-      <c r="BF103" t="s">
+      <c r="BF103" s="1" t="s">
         <v>130</v>
       </c>
       <c r="BG103" s="1"/>
@@ -12582,7 +12649,7 @@
       <c r="CG103" s="1"/>
     </row>
     <row r="104" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A104" s="5">
+      <c r="A104" s="4">
         <v>101</v>
       </c>
       <c r="B104" s="1" t="s">
@@ -12628,7 +12695,9 @@
       <c r="AN104" s="1"/>
       <c r="AO104" s="1"/>
       <c r="AP104" s="1"/>
-      <c r="AQ104" s="1"/>
+      <c r="AQ104" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="AR104" s="1"/>
       <c r="AS104" s="1"/>
       <c r="AT104" s="1"/>
@@ -12645,7 +12714,7 @@
       <c r="BC104" s="1"/>
       <c r="BD104" s="1"/>
       <c r="BE104" s="1"/>
-      <c r="BF104" t="s">
+      <c r="BF104" s="1" t="s">
         <v>131</v>
       </c>
       <c r="BG104" s="1"/>
@@ -12677,7 +12746,7 @@
       <c r="CG104" s="1"/>
     </row>
     <row r="105" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A105" s="5">
+      <c r="A105" s="4">
         <v>102</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -12740,7 +12809,7 @@
       <c r="BC105" s="1"/>
       <c r="BD105" s="1"/>
       <c r="BE105" s="1"/>
-      <c r="BF105" t="s">
+      <c r="BF105" s="1" t="s">
         <v>132</v>
       </c>
       <c r="BG105" s="1"/>
@@ -12772,7 +12841,7 @@
       <c r="CG105" s="1"/>
     </row>
     <row r="106" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A106" s="5">
+      <c r="A106" s="4">
         <v>103</v>
       </c>
       <c r="B106" s="1" t="s">
@@ -12885,7 +12954,7 @@
       <c r="BE106" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="BF106" t="s">
+      <c r="BF106" s="1" t="s">
         <v>133</v>
       </c>
       <c r="BG106" s="1"/>
@@ -12917,7 +12986,7 @@
       <c r="CG106" s="1"/>
     </row>
     <row r="107" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A107" s="5">
+      <c r="A107" s="4">
         <v>104</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -12986,7 +13055,7 @@
       </c>
       <c r="BD107" s="1"/>
       <c r="BE107" s="1"/>
-      <c r="BF107" t="s">
+      <c r="BF107" s="1" t="s">
         <v>134</v>
       </c>
       <c r="BG107" s="1"/>
@@ -13018,7 +13087,7 @@
       <c r="CG107" s="1"/>
     </row>
     <row r="108" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A108" s="5">
+      <c r="A108" s="4">
         <v>105</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -13133,7 +13202,7 @@
       <c r="BE108" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BF108" t="s">
+      <c r="BF108" s="1" t="s">
         <v>136</v>
       </c>
       <c r="BG108" s="1"/>
@@ -13165,7 +13234,7 @@
       <c r="CG108" s="1"/>
     </row>
     <row r="109" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A109" s="5">
+      <c r="A109" s="4">
         <v>106</v>
       </c>
       <c r="B109" s="1"/>
@@ -13232,6 +13301,7 @@
       <c r="BC109" s="1"/>
       <c r="BD109" s="1"/>
       <c r="BE109" s="1"/>
+      <c r="BF109" s="1"/>
       <c r="BG109" s="1"/>
       <c r="BH109" s="1"/>
       <c r="BI109" s="1"/>
@@ -13277,7 +13347,7 @@
       <c r="CG109" s="1"/>
     </row>
     <row r="110" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A110" s="5">
+      <c r="A110" s="4">
         <v>107</v>
       </c>
       <c r="B110" s="1"/>
@@ -13360,6 +13430,7 @@
       <c r="BC110" s="1"/>
       <c r="BD110" s="1"/>
       <c r="BE110" s="1"/>
+      <c r="BF110" s="1"/>
       <c r="BG110" s="1"/>
       <c r="BH110" s="1"/>
       <c r="BI110" s="1">
@@ -13423,7 +13494,7 @@
       </c>
     </row>
     <row r="111" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A111" s="5">
+      <c r="A111" s="4">
         <v>108</v>
       </c>
       <c r="B111" s="1"/>
@@ -13506,6 +13577,7 @@
       <c r="BC111" s="1"/>
       <c r="BD111" s="1"/>
       <c r="BE111" s="1"/>
+      <c r="BF111" s="1"/>
       <c r="BG111" s="1"/>
       <c r="BH111" s="1"/>
       <c r="BI111" s="1">
@@ -13569,7 +13641,7 @@
       </c>
     </row>
     <row r="112" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A112" s="5">
+      <c r="A112" s="4">
         <v>109</v>
       </c>
       <c r="B112" s="1"/>
@@ -13634,6 +13706,7 @@
       <c r="BC112" s="1"/>
       <c r="BD112" s="1"/>
       <c r="BE112" s="1"/>
+      <c r="BF112" s="1"/>
       <c r="BG112" s="1"/>
       <c r="BH112" s="1"/>
       <c r="BI112" s="1"/>
@@ -13665,7 +13738,7 @@
       </c>
     </row>
     <row r="113" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A113" s="5">
+      <c r="A113" s="4">
         <v>110</v>
       </c>
       <c r="B113" s="1"/>
@@ -13750,6 +13823,7 @@
       <c r="BC113" s="1"/>
       <c r="BD113" s="1"/>
       <c r="BE113" s="1"/>
+      <c r="BF113" s="1"/>
       <c r="BG113" s="1"/>
       <c r="BH113" s="1"/>
       <c r="BI113" s="1"/>
@@ -13781,7 +13855,7 @@
       <c r="CG113" s="1"/>
     </row>
     <row r="114" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A114" s="5">
+      <c r="A114" s="4">
         <v>111</v>
       </c>
       <c r="B114" s="1"/>
@@ -13842,6 +13916,7 @@
       <c r="BC114" s="1"/>
       <c r="BD114" s="1"/>
       <c r="BE114" s="1"/>
+      <c r="BF114" s="1"/>
       <c r="BG114" s="1"/>
       <c r="BH114" s="1"/>
       <c r="BI114" s="1"/>
@@ -13871,7 +13946,7 @@
       <c r="CG114" s="1"/>
     </row>
     <row r="115" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A115" s="5">
+      <c r="A115" s="4">
         <v>112</v>
       </c>
       <c r="B115" s="1"/>
@@ -13932,6 +14007,7 @@
       <c r="BC115" s="1"/>
       <c r="BD115" s="1"/>
       <c r="BE115" s="1"/>
+      <c r="BF115" s="1"/>
       <c r="BG115" s="1"/>
       <c r="BH115" s="1"/>
       <c r="BI115" s="1"/>
@@ -13961,7 +14037,7 @@
       <c r="CG115" s="1"/>
     </row>
     <row r="116" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A116" s="5">
+      <c r="A116" s="4">
         <v>113</v>
       </c>
       <c r="B116" s="1"/>
@@ -14024,6 +14100,7 @@
       <c r="BC116" s="1"/>
       <c r="BD116" s="1"/>
       <c r="BE116" s="1"/>
+      <c r="BF116" s="1"/>
       <c r="BG116" s="1"/>
       <c r="BH116" s="1"/>
       <c r="BI116" s="1"/>
@@ -14053,7 +14130,7 @@
       <c r="CG116" s="1"/>
     </row>
     <row r="117" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A117" s="5">
+      <c r="A117" s="4">
         <v>114</v>
       </c>
       <c r="B117" s="1"/>
@@ -14122,6 +14199,7 @@
       <c r="BC117" s="1"/>
       <c r="BD117" s="1"/>
       <c r="BE117" s="1"/>
+      <c r="BF117" s="1"/>
       <c r="BG117" s="1"/>
       <c r="BH117" s="1"/>
       <c r="BI117" s="1"/>
@@ -14165,7 +14243,7 @@
       <c r="CG117" s="1"/>
     </row>
     <row r="118" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A118" s="5">
+      <c r="A118" s="4">
         <v>115</v>
       </c>
       <c r="B118" s="1" t="s">
@@ -14234,7 +14312,7 @@
       </c>
       <c r="BD118" s="1"/>
       <c r="BE118" s="1"/>
-      <c r="BF118" t="s">
+      <c r="BF118" s="1" t="s">
         <v>146</v>
       </c>
       <c r="BG118" s="1"/>
@@ -14266,7 +14344,7 @@
       <c r="CG118" s="1"/>
     </row>
     <row r="119" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A119" s="5">
+      <c r="A119" s="4">
         <v>116</v>
       </c>
       <c r="B119" s="1" t="s">
@@ -14379,7 +14457,7 @@
       <c r="BE119" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BF119" t="s">
+      <c r="BF119" s="1" t="s">
         <v>147</v>
       </c>
       <c r="BG119" s="1"/>
@@ -14411,7 +14489,7 @@
       <c r="CG119" s="1"/>
     </row>
     <row r="120" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A120" s="5">
+      <c r="A120" s="4">
         <v>117</v>
       </c>
       <c r="B120" s="1" t="s">
@@ -14480,7 +14558,7 @@
       </c>
       <c r="BD120" s="1"/>
       <c r="BE120" s="1"/>
-      <c r="BF120" t="s">
+      <c r="BF120" s="1" t="s">
         <v>148</v>
       </c>
       <c r="BG120" s="1"/>
@@ -14512,7 +14590,7 @@
       <c r="CG120" s="1"/>
     </row>
     <row r="121" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A121" s="5">
+      <c r="A121" s="4">
         <v>118</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -14625,7 +14703,7 @@
       <c r="BE121" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="BF121" t="s">
+      <c r="BF121" s="1" t="s">
         <v>149</v>
       </c>
       <c r="BG121" s="1"/>
@@ -14657,7 +14735,7 @@
       <c r="CG121" s="1"/>
     </row>
     <row r="122" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A122" s="5">
+      <c r="A122" s="4">
         <v>119</v>
       </c>
       <c r="B122" s="1"/>
@@ -14718,6 +14796,7 @@
       <c r="BC122" s="1"/>
       <c r="BD122" s="1"/>
       <c r="BE122" s="1"/>
+      <c r="BF122" s="1"/>
       <c r="BG122" s="1"/>
       <c r="BH122" s="1"/>
       <c r="BI122" s="1"/>
@@ -14747,7 +14826,7 @@
       <c r="CG122" s="1"/>
     </row>
     <row r="123" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A123" s="5">
+      <c r="A123" s="4">
         <v>120</v>
       </c>
       <c r="B123" s="1" t="s">
@@ -14810,7 +14889,7 @@
       <c r="BC123" s="1"/>
       <c r="BD123" s="1"/>
       <c r="BE123" s="1"/>
-      <c r="BF123" t="s">
+      <c r="BF123" s="1" t="s">
         <v>151</v>
       </c>
       <c r="BG123" s="1"/>
@@ -14842,7 +14921,7 @@
       <c r="CG123" s="1"/>
     </row>
     <row r="124" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A124" s="5">
+      <c r="A124" s="4">
         <v>121</v>
       </c>
       <c r="B124" s="1" t="s">
@@ -14909,7 +14988,7 @@
       <c r="BC124" s="1"/>
       <c r="BD124" s="1"/>
       <c r="BE124" s="1"/>
-      <c r="BF124" t="s">
+      <c r="BF124" s="1" t="s">
         <v>153</v>
       </c>
       <c r="BG124" s="1"/>
@@ -14943,7 +15022,7 @@
       <c r="CG124" s="1"/>
     </row>
     <row r="125" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A125" s="5">
+      <c r="A125" s="4">
         <v>122</v>
       </c>
       <c r="B125" s="1"/>
@@ -15024,6 +15103,7 @@
       <c r="BC125" s="1"/>
       <c r="BD125" s="1"/>
       <c r="BE125" s="1"/>
+      <c r="BF125" s="1"/>
       <c r="BG125" s="1"/>
       <c r="BH125" s="1">
         <v>138</v>
@@ -15087,7 +15167,7 @@
       </c>
     </row>
     <row r="126" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A126" s="5">
+      <c r="A126" s="4">
         <v>123</v>
       </c>
       <c r="B126" s="1" t="s">
@@ -15152,7 +15232,7 @@
       <c r="BC126" s="1"/>
       <c r="BD126" s="1"/>
       <c r="BE126" s="1"/>
-      <c r="BF126" t="s">
+      <c r="BF126" s="1" t="s">
         <v>155</v>
       </c>
       <c r="BG126" s="1"/>
@@ -15186,7 +15266,7 @@
       <c r="CG126" s="1"/>
     </row>
     <row r="127" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A127" s="5">
+      <c r="A127" s="4">
         <v>124</v>
       </c>
       <c r="B127" s="1"/>
@@ -15247,6 +15327,7 @@
       <c r="BC127" s="1"/>
       <c r="BD127" s="1"/>
       <c r="BE127" s="1"/>
+      <c r="BF127" s="1"/>
       <c r="BG127" s="1"/>
       <c r="BH127" s="1"/>
       <c r="BI127" s="1"/>
@@ -15276,7 +15357,7 @@
       <c r="CG127" s="1"/>
     </row>
     <row r="128" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A128" s="5">
+      <c r="A128" s="4">
         <v>125</v>
       </c>
       <c r="B128" s="1"/>
@@ -15343,6 +15424,7 @@
       <c r="BC128" s="1"/>
       <c r="BD128" s="1"/>
       <c r="BE128" s="1"/>
+      <c r="BF128" s="1"/>
       <c r="BG128" s="1"/>
       <c r="BH128" s="1"/>
       <c r="BI128" s="1"/>
@@ -15386,7 +15468,7 @@
       <c r="CG128" s="1"/>
     </row>
     <row r="129" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A129" s="5">
+      <c r="A129" s="4">
         <v>126</v>
       </c>
       <c r="B129" s="1"/>
@@ -15453,6 +15535,7 @@
       <c r="BC129" s="1"/>
       <c r="BD129" s="1"/>
       <c r="BE129" s="1"/>
+      <c r="BF129" s="1"/>
       <c r="BG129" s="1"/>
       <c r="BH129" s="1"/>
       <c r="BI129" s="1"/>
@@ -15496,7 +15579,7 @@
       <c r="CG129" s="1"/>
     </row>
     <row r="130" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A130" s="5">
+      <c r="A130" s="4">
         <v>127</v>
       </c>
       <c r="B130" s="1"/>
@@ -15563,6 +15646,7 @@
       <c r="BC130" s="1"/>
       <c r="BD130" s="1"/>
       <c r="BE130" s="1"/>
+      <c r="BF130" s="1"/>
       <c r="BG130" s="1"/>
       <c r="BH130" s="1"/>
       <c r="BI130" s="1"/>
@@ -15608,7 +15692,7 @@
       <c r="CG130" s="1"/>
     </row>
     <row r="131" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A131" s="5">
+      <c r="A131" s="4">
         <v>128</v>
       </c>
       <c r="B131" s="1" t="s">
@@ -15677,7 +15761,7 @@
       </c>
       <c r="BD131" s="1"/>
       <c r="BE131" s="1"/>
-      <c r="BF131" t="s">
+      <c r="BF131" s="1" t="s">
         <v>158</v>
       </c>
       <c r="BG131" s="1"/>
@@ -15709,7 +15793,7 @@
       <c r="CG131" s="1"/>
     </row>
     <row r="132" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A132" s="5">
+      <c r="A132" s="4">
         <v>129</v>
       </c>
       <c r="B132" s="1" t="s">
@@ -15778,7 +15862,7 @@
       </c>
       <c r="BD132" s="1"/>
       <c r="BE132" s="1"/>
-      <c r="BF132" t="s">
+      <c r="BF132" s="1" t="s">
         <v>159</v>
       </c>
       <c r="BG132" s="1"/>
@@ -15810,7 +15894,7 @@
       <c r="CG132" s="1"/>
     </row>
     <row r="133" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A133" s="5">
+      <c r="A133" s="4">
         <v>130</v>
       </c>
       <c r="B133" s="1" t="s">
@@ -15881,7 +15965,7 @@
       </c>
       <c r="BD133" s="1"/>
       <c r="BE133" s="1"/>
-      <c r="BF133" t="s">
+      <c r="BF133" s="1" t="s">
         <v>160</v>
       </c>
       <c r="BG133" s="1"/>
@@ -15913,7 +15997,7 @@
       <c r="CG133" s="1"/>
     </row>
     <row r="134" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A134" s="5">
+      <c r="A134" s="4">
         <v>131</v>
       </c>
       <c r="B134" s="1"/>
@@ -15976,6 +16060,7 @@
       <c r="BC134" s="1"/>
       <c r="BD134" s="1"/>
       <c r="BE134" s="1"/>
+      <c r="BF134" s="1"/>
       <c r="BG134" s="1"/>
       <c r="BH134" s="1"/>
       <c r="BI134" s="1"/>
@@ -16011,7 +16096,7 @@
       <c r="CG134" s="1"/>
     </row>
     <row r="135" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A135" s="5">
+      <c r="A135" s="4">
         <v>132</v>
       </c>
       <c r="B135" s="1"/>
@@ -16072,6 +16157,7 @@
       <c r="BC135" s="1"/>
       <c r="BD135" s="1"/>
       <c r="BE135" s="1"/>
+      <c r="BF135" s="1"/>
       <c r="BG135" s="1"/>
       <c r="BH135" s="1"/>
       <c r="BI135" s="1"/>
@@ -16101,7 +16187,7 @@
       <c r="CG135" s="1"/>
     </row>
     <row r="136" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A136" s="5">
+      <c r="A136" s="4">
         <v>133</v>
       </c>
       <c r="B136" s="1"/>
@@ -16162,6 +16248,7 @@
       <c r="BC136" s="1"/>
       <c r="BD136" s="1"/>
       <c r="BE136" s="1"/>
+      <c r="BF136" s="1"/>
       <c r="BG136" s="1"/>
       <c r="BH136" s="1"/>
       <c r="BI136" s="1"/>
@@ -16191,7 +16278,7 @@
       <c r="CG136" s="1"/>
     </row>
     <row r="137" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A137" s="5">
+      <c r="A137" s="4">
         <v>134</v>
       </c>
       <c r="B137" s="1" t="s">
@@ -16258,7 +16345,7 @@
       <c r="BC137" s="1"/>
       <c r="BD137" s="1"/>
       <c r="BE137" s="1"/>
-      <c r="BF137" t="s">
+      <c r="BF137" s="1" t="s">
         <v>163</v>
       </c>
       <c r="BG137" s="1"/>
@@ -16290,7 +16377,7 @@
       <c r="CG137" s="1"/>
     </row>
     <row r="138" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A138" s="5">
+      <c r="A138" s="4">
         <v>135</v>
       </c>
       <c r="B138" s="1" t="s">
@@ -16357,7 +16444,7 @@
       <c r="BC138" s="1"/>
       <c r="BD138" s="1"/>
       <c r="BE138" s="1"/>
-      <c r="BF138" t="s">
+      <c r="BF138" s="1" t="s">
         <v>164</v>
       </c>
       <c r="BG138" s="1"/>
@@ -16389,7 +16476,7 @@
       <c r="CG138" s="1"/>
     </row>
     <row r="139" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A139" s="5">
+      <c r="A139" s="4">
         <v>136</v>
       </c>
       <c r="B139" s="1" t="s">
@@ -16454,7 +16541,7 @@
       <c r="BC139" s="1"/>
       <c r="BD139" s="1"/>
       <c r="BE139" s="1"/>
-      <c r="BF139" t="s">
+      <c r="BF139" s="1" t="s">
         <v>155</v>
       </c>
       <c r="BG139" s="1"/>
@@ -16488,7 +16575,7 @@
       <c r="CG139" s="1"/>
     </row>
     <row r="140" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A140" s="5">
+      <c r="A140" s="4">
         <v>137</v>
       </c>
       <c r="B140" s="1"/>
@@ -16555,6 +16642,7 @@
       <c r="BC140" s="1"/>
       <c r="BD140" s="1"/>
       <c r="BE140" s="1"/>
+      <c r="BF140" s="1"/>
       <c r="BG140" s="1"/>
       <c r="BH140" s="1"/>
       <c r="BI140" s="1"/>
@@ -16600,7 +16688,7 @@
       <c r="CG140" s="1"/>
     </row>
     <row r="141" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A141" s="5">
+      <c r="A141" s="4">
         <v>138</v>
       </c>
       <c r="B141" s="1" t="s">
@@ -16667,7 +16755,7 @@
       <c r="BC141" s="1"/>
       <c r="BD141" s="1"/>
       <c r="BE141" s="1"/>
-      <c r="BF141" t="s">
+      <c r="BF141" s="1" t="s">
         <v>165</v>
       </c>
       <c r="BG141" s="1"/>
@@ -16699,7 +16787,7 @@
       <c r="CG141" s="1"/>
     </row>
     <row r="142" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A142" s="5">
+      <c r="A142" s="4">
         <v>139</v>
       </c>
       <c r="B142" s="1" t="s">
@@ -16762,7 +16850,7 @@
       <c r="BC142" s="1"/>
       <c r="BD142" s="1"/>
       <c r="BE142" s="1"/>
-      <c r="BF142" t="s">
+      <c r="BF142" s="1" t="s">
         <v>166</v>
       </c>
       <c r="BG142" s="1"/>
@@ -16794,7 +16882,7 @@
       <c r="CG142" s="1"/>
     </row>
     <row r="143" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A143" s="5">
+      <c r="A143" s="4">
         <v>140</v>
       </c>
       <c r="B143" s="1"/>
@@ -16861,6 +16949,7 @@
       <c r="BC143" s="1"/>
       <c r="BD143" s="1"/>
       <c r="BE143" s="1"/>
+      <c r="BF143" s="1"/>
       <c r="BG143" s="1"/>
       <c r="BH143" s="1"/>
       <c r="BI143" s="1"/>
@@ -16906,7 +16995,7 @@
       <c r="CG143" s="1"/>
     </row>
     <row r="144" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A144" s="5">
+      <c r="A144" s="4">
         <v>141</v>
       </c>
       <c r="B144" s="1"/>
@@ -16989,6 +17078,7 @@
       <c r="BC144" s="1"/>
       <c r="BD144" s="1"/>
       <c r="BE144" s="1"/>
+      <c r="BF144" s="1"/>
       <c r="BG144" s="1"/>
       <c r="BH144" s="1"/>
       <c r="BI144" s="1">
@@ -17052,7 +17142,7 @@
       </c>
     </row>
     <row r="145" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A145" s="5">
+      <c r="A145" s="4">
         <v>142</v>
       </c>
       <c r="B145" s="1"/>
@@ -17113,6 +17203,7 @@
       <c r="BC145" s="1"/>
       <c r="BD145" s="1"/>
       <c r="BE145" s="1"/>
+      <c r="BF145" s="1"/>
       <c r="BG145" s="1"/>
       <c r="BH145" s="1"/>
       <c r="BI145" s="1"/>
@@ -17142,7 +17233,7 @@
       <c r="CG145" s="1"/>
     </row>
     <row r="146" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A146" s="5">
+      <c r="A146" s="4">
         <v>143</v>
       </c>
       <c r="B146" s="1"/>
@@ -17203,6 +17294,7 @@
       </c>
       <c r="BD146" s="1"/>
       <c r="BE146" s="1"/>
+      <c r="BF146" s="1"/>
       <c r="BG146" s="1"/>
       <c r="BH146" s="1"/>
       <c r="BI146" s="1"/>
@@ -17232,7 +17324,7 @@
       <c r="CG146" s="1"/>
     </row>
     <row r="147" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A147" s="5">
+      <c r="A147" s="4">
         <v>144</v>
       </c>
       <c r="B147" s="1"/>
@@ -17295,6 +17387,7 @@
       <c r="BC147" s="1"/>
       <c r="BD147" s="1"/>
       <c r="BE147" s="1"/>
+      <c r="BF147" s="1"/>
       <c r="BG147" s="1"/>
       <c r="BH147" s="1"/>
       <c r="BI147" s="1"/>
@@ -17324,7 +17417,7 @@
       <c r="CG147" s="1"/>
     </row>
     <row r="148" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A148" s="5">
+      <c r="A148" s="4">
         <v>145</v>
       </c>
       <c r="B148" s="1"/>
@@ -17387,6 +17480,7 @@
       <c r="BC148" s="1"/>
       <c r="BD148" s="1"/>
       <c r="BE148" s="1"/>
+      <c r="BF148" s="1"/>
       <c r="BG148" s="1"/>
       <c r="BH148" s="1"/>
       <c r="BI148" s="1"/>
@@ -17416,7 +17510,7 @@
       <c r="CG148" s="1"/>
     </row>
     <row r="149" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A149" s="5">
+      <c r="A149" s="4">
         <v>146</v>
       </c>
       <c r="B149" s="1"/>
@@ -17477,6 +17571,7 @@
       <c r="BC149" s="1"/>
       <c r="BD149" s="1"/>
       <c r="BE149" s="1"/>
+      <c r="BF149" s="1"/>
       <c r="BG149" s="1"/>
       <c r="BH149" s="1"/>
       <c r="BI149" s="1"/>
@@ -17506,7 +17601,7 @@
       <c r="CG149" s="1"/>
     </row>
     <row r="150" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A150" s="5">
+      <c r="A150" s="4">
         <v>147</v>
       </c>
       <c r="B150" s="1"/>
@@ -17589,6 +17684,7 @@
       <c r="BC150" s="1"/>
       <c r="BD150" s="1"/>
       <c r="BE150" s="1"/>
+      <c r="BF150" s="1"/>
       <c r="BG150" s="1"/>
       <c r="BH150" s="1"/>
       <c r="BI150" s="1">
@@ -17652,7 +17748,7 @@
       </c>
     </row>
     <row r="151" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A151" s="5">
+      <c r="A151" s="4">
         <v>148</v>
       </c>
       <c r="B151" s="1" t="s">
@@ -17715,7 +17811,7 @@
       <c r="BC151" s="1"/>
       <c r="BD151" s="1"/>
       <c r="BE151" s="1"/>
-      <c r="BF151" t="s">
+      <c r="BF151" s="1" t="s">
         <v>173</v>
       </c>
       <c r="BG151" s="1"/>
@@ -17747,7 +17843,7 @@
       <c r="CG151" s="1"/>
     </row>
     <row r="152" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A152" s="5">
+      <c r="A152" s="4">
         <v>149</v>
       </c>
       <c r="B152" s="1"/>
@@ -17808,6 +17904,7 @@
       <c r="BC152" s="1"/>
       <c r="BD152" s="1"/>
       <c r="BE152" s="1"/>
+      <c r="BF152" s="1"/>
       <c r="BG152" s="1"/>
       <c r="BH152" s="1"/>
       <c r="BI152" s="1"/>
@@ -17837,7 +17934,7 @@
       <c r="CG152" s="1"/>
     </row>
     <row r="153" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A153" s="5">
+      <c r="A153" s="4">
         <v>150</v>
       </c>
       <c r="B153" s="1"/>
@@ -17898,6 +17995,7 @@
       <c r="BC153" s="1"/>
       <c r="BD153" s="1"/>
       <c r="BE153" s="1"/>
+      <c r="BF153" s="1"/>
       <c r="BG153" s="1"/>
       <c r="BH153" s="1"/>
       <c r="BI153" s="1"/>
@@ -17927,7 +18025,7 @@
       <c r="CG153" s="1"/>
     </row>
     <row r="154" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A154" s="5">
+      <c r="A154" s="4">
         <v>151</v>
       </c>
       <c r="B154" s="1" t="s">
@@ -17990,7 +18088,7 @@
       <c r="BC154" s="1"/>
       <c r="BD154" s="1"/>
       <c r="BE154" s="1"/>
-      <c r="BF154" t="s">
+      <c r="BF154" s="1" t="s">
         <v>176</v>
       </c>
       <c r="BG154" s="1"/>
@@ -18022,7 +18120,7 @@
       <c r="CG154" s="1"/>
     </row>
     <row r="155" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A155" s="5">
+      <c r="A155" s="4">
         <v>152</v>
       </c>
       <c r="B155" s="1"/>
@@ -18083,6 +18181,7 @@
       <c r="BC155" s="1"/>
       <c r="BD155" s="1"/>
       <c r="BE155" s="1"/>
+      <c r="BF155" s="1"/>
       <c r="BG155" s="1"/>
       <c r="BH155" s="1"/>
       <c r="BI155" s="1"/>
@@ -18112,7 +18211,7 @@
       <c r="CG155" s="1"/>
     </row>
     <row r="156" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A156" s="5">
+      <c r="A156" s="4">
         <v>153</v>
       </c>
       <c r="B156" s="1"/>
@@ -18173,6 +18272,7 @@
       <c r="BC156" s="1"/>
       <c r="BD156" s="1"/>
       <c r="BE156" s="1"/>
+      <c r="BF156" s="1"/>
       <c r="BG156" s="1"/>
       <c r="BH156" s="1"/>
       <c r="BI156" s="1"/>
@@ -18202,7 +18302,7 @@
       <c r="CG156" s="1"/>
     </row>
     <row r="157" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A157" s="5">
+      <c r="A157" s="4">
         <v>154</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -18273,7 +18373,7 @@
       </c>
       <c r="BD157" s="1"/>
       <c r="BE157" s="1"/>
-      <c r="BF157" t="s">
+      <c r="BF157" s="1" t="s">
         <v>179</v>
       </c>
       <c r="BG157" s="1"/>
@@ -18305,7 +18405,7 @@
       <c r="CG157" s="1"/>
     </row>
     <row r="158" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A158" s="5">
+      <c r="A158" s="4">
         <v>155</v>
       </c>
       <c r="B158" s="1"/>
@@ -18368,6 +18468,7 @@
       <c r="BC158" s="1"/>
       <c r="BD158" s="1"/>
       <c r="BE158" s="1"/>
+      <c r="BF158" s="1"/>
       <c r="BG158" s="1"/>
       <c r="BH158" s="1"/>
       <c r="BI158" s="1"/>
@@ -18403,7 +18504,7 @@
       <c r="CG158" s="1"/>
     </row>
     <row r="159" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A159" s="5">
+      <c r="A159" s="4">
         <v>156</v>
       </c>
       <c r="B159" s="1"/>
@@ -18486,6 +18587,7 @@
       <c r="BC159" s="1"/>
       <c r="BD159" s="1"/>
       <c r="BE159" s="1"/>
+      <c r="BF159" s="1"/>
       <c r="BG159" s="1"/>
       <c r="BH159" s="1"/>
       <c r="BI159" s="1">
@@ -18549,7 +18651,7 @@
       </c>
     </row>
     <row r="160" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A160" s="5">
+      <c r="A160" s="4">
         <v>157</v>
       </c>
       <c r="B160" s="1" t="s">
@@ -18612,7 +18714,7 @@
       <c r="BC160" s="1"/>
       <c r="BD160" s="1"/>
       <c r="BE160" s="1"/>
-      <c r="BF160" t="s">
+      <c r="BF160" s="1" t="s">
         <v>180</v>
       </c>
       <c r="BG160" s="1"/>
@@ -18644,7 +18746,7 @@
       <c r="CG160" s="1"/>
     </row>
     <row r="161" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A161" s="5">
+      <c r="A161" s="4">
         <v>158</v>
       </c>
       <c r="B161" s="1"/>
@@ -18727,6 +18829,7 @@
       <c r="BC161" s="1"/>
       <c r="BD161" s="1"/>
       <c r="BE161" s="1"/>
+      <c r="BF161" s="1"/>
       <c r="BG161" s="1"/>
       <c r="BH161" s="1"/>
       <c r="BI161" s="1">
@@ -18790,7 +18893,7 @@
       </c>
     </row>
     <row r="162" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A162" s="5">
+      <c r="A162" s="4">
         <v>159</v>
       </c>
       <c r="B162" s="1"/>
@@ -18873,6 +18976,7 @@
       <c r="BC162" s="1"/>
       <c r="BD162" s="1"/>
       <c r="BE162" s="1"/>
+      <c r="BF162" s="1"/>
       <c r="BG162" s="1"/>
       <c r="BH162" s="1"/>
       <c r="BI162" s="1">
@@ -18936,7 +19040,7 @@
       </c>
     </row>
     <row r="163" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A163" s="5">
+      <c r="A163" s="4">
         <v>160</v>
       </c>
       <c r="B163" s="1"/>
@@ -19019,6 +19123,7 @@
       <c r="BC163" s="1"/>
       <c r="BD163" s="1"/>
       <c r="BE163" s="1"/>
+      <c r="BF163" s="1"/>
       <c r="BG163" s="1"/>
       <c r="BH163" s="1"/>
       <c r="BI163" s="1">
@@ -19082,7 +19187,7 @@
       </c>
     </row>
     <row r="164" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A164" s="5">
+      <c r="A164" s="4">
         <v>161</v>
       </c>
       <c r="B164" s="1"/>
@@ -19165,6 +19270,7 @@
       <c r="BC164" s="1"/>
       <c r="BD164" s="1"/>
       <c r="BE164" s="1"/>
+      <c r="BF164" s="1"/>
       <c r="BG164" s="1"/>
       <c r="BH164" s="1"/>
       <c r="BI164" s="1">
@@ -19228,7 +19334,7 @@
       </c>
     </row>
     <row r="165" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A165" s="5">
+      <c r="A165" s="4">
         <v>162</v>
       </c>
       <c r="B165" s="1"/>
@@ -19289,6 +19395,7 @@
       <c r="BC165" s="1"/>
       <c r="BD165" s="1"/>
       <c r="BE165" s="1"/>
+      <c r="BF165" s="1"/>
       <c r="BG165" s="1"/>
       <c r="BH165" s="1"/>
       <c r="BI165" s="1"/>
@@ -19318,7 +19425,7 @@
       <c r="CG165" s="1"/>
     </row>
     <row r="166" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A166" s="5">
+      <c r="A166" s="4">
         <v>163</v>
       </c>
       <c r="B166" s="1" t="s">
@@ -19381,7 +19488,7 @@
       <c r="BC166" s="1"/>
       <c r="BD166" s="1"/>
       <c r="BE166" s="1"/>
-      <c r="BF166" t="s">
+      <c r="BF166" s="1" t="s">
         <v>182</v>
       </c>
       <c r="BG166" s="1"/>
@@ -19413,7 +19520,7 @@
       <c r="CG166" s="1"/>
     </row>
     <row r="167" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A167" s="5">
+      <c r="A167" s="4">
         <v>164</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -19480,7 +19587,7 @@
       <c r="BC167" s="1"/>
       <c r="BD167" s="1"/>
       <c r="BE167" s="1"/>
-      <c r="BF167" t="s">
+      <c r="BF167" s="1" t="s">
         <v>153</v>
       </c>
       <c r="BG167" s="1"/>
@@ -19514,7 +19621,7 @@
       <c r="CG167" s="1"/>
     </row>
     <row r="168" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A168" s="5">
+      <c r="A168" s="4">
         <v>165</v>
       </c>
       <c r="B168" s="1" t="s">
@@ -19577,7 +19684,7 @@
       <c r="BC168" s="1"/>
       <c r="BD168" s="1"/>
       <c r="BE168" s="1"/>
-      <c r="BF168" t="s">
+      <c r="BF168" s="1" t="s">
         <v>183</v>
       </c>
       <c r="BG168" s="1"/>
@@ -19609,7 +19716,7 @@
       <c r="CG168" s="1"/>
     </row>
     <row r="169" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A169" s="5">
+      <c r="A169" s="4">
         <v>166</v>
       </c>
       <c r="B169" s="1" t="s">
@@ -19672,7 +19779,7 @@
       <c r="BC169" s="1"/>
       <c r="BD169" s="1"/>
       <c r="BE169" s="1"/>
-      <c r="BF169" t="s">
+      <c r="BF169" s="1" t="s">
         <v>184</v>
       </c>
       <c r="BG169" s="1"/>
@@ -19704,7 +19811,7 @@
       <c r="CG169" s="1"/>
     </row>
     <row r="170" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A170" s="5">
+      <c r="A170" s="4">
         <v>167</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -19767,7 +19874,7 @@
       <c r="BC170" s="1"/>
       <c r="BD170" s="1"/>
       <c r="BE170" s="1"/>
-      <c r="BF170" t="s">
+      <c r="BF170" s="1" t="s">
         <v>185</v>
       </c>
       <c r="BG170" s="1"/>
@@ -19799,7 +19906,7 @@
       <c r="CG170" s="1"/>
     </row>
     <row r="171" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A171" s="5">
+      <c r="A171" s="4">
         <v>168</v>
       </c>
       <c r="B171" s="1" t="s">
@@ -19870,7 +19977,7 @@
       </c>
       <c r="BD171" s="1"/>
       <c r="BE171" s="1"/>
-      <c r="BF171" t="s">
+      <c r="BF171" s="1" t="s">
         <v>186</v>
       </c>
       <c r="BG171" s="1"/>
@@ -19902,7 +20009,7 @@
       <c r="CG171" s="1"/>
     </row>
     <row r="172" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A172" s="5">
+      <c r="A172" s="4">
         <v>169</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -19967,7 +20074,7 @@
       <c r="BC172" s="1"/>
       <c r="BD172" s="1"/>
       <c r="BE172" s="1"/>
-      <c r="BF172" t="s">
+      <c r="BF172" s="1" t="s">
         <v>187</v>
       </c>
       <c r="BG172" s="1"/>

</xml_diff>